<commit_message>
Deployed 2d689e95 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/en/Manual/source/tab/connectors.xlsx
+++ b/en/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="66"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -73,9 +73,11 @@
     <sheet name="X4_ACIN_4pin_TGS560_25" sheetId="63" state="visible" r:id="rId65"/>
     <sheet name="X1_DC_6pin_TGS560_25" sheetId="64" state="visible" r:id="rId66"/>
     <sheet name="X5_RBR_3pin_TGS560_25" sheetId="65" state="visible" r:id="rId67"/>
+    <sheet name="X0a_48-100-xyz" sheetId="66" state="visible" r:id="rId68"/>
+    <sheet name="X0b_48-100-xyz" sheetId="67" state="visible" r:id="rId69"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId68"/>
+    <externalReference r:id="rId70"/>
   </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -87,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2066" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="545">
   <si>
     <t xml:space="preserve">This is a workbook with source tables of TGZ/TGS connector descriptions in English. Each sheet corresponds to one unique connector type. Since connectors are often repeated within TGZ (typically those on the control board), they are only listed once. I.e. E.g. IO connector 22pin weidmuller B2CF is used over and over again, so it is only listed here once as "X8_IO_22pin_B2CF"</t>
   </si>
@@ -1717,6 +1719,48 @@
   </si>
   <si>
     <t xml:space="preserve">Brake resistor select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor phase U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 ~ 1/0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor phase V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor phase W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+DC bus input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-DC bus input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static brake GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 ~ 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static brake +24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static brake – terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static brake + terminal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 V control supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External P1000</t>
   </si>
 </sst>
 </file>
@@ -1962,6 +2006,7 @@
       <sheetName val="rozcestnik"/>
       <sheetName val="conns"/>
       <sheetName val="X1_24V_5pin_BCZ"/>
+      <sheetName val="X1_24V_5pin_BCZ_D4850"/>
       <sheetName val="X2_48_DC_1778065"/>
       <sheetName val="X8_IO_22pin_B2CF"/>
       <sheetName val="X10_CAN_4pin_B2CF"/>
@@ -2847,6 +2892,7 @@
       <sheetData sheetId="61"/>
       <sheetData sheetId="62"/>
       <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -12989,7 +13035,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13518,7 +13564,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14800,7 +14846,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -17694,7 +17740,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17808,7 +17854,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17891,7 +17937,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19315,6 +19361,354 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.85"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.93"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="1"/>
+      <c r="C21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="1"/>
+      <c r="C22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1"/>
+      <c r="C23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1"/>
+      <c r="C24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1"/>
+      <c r="C25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">

</xml_diff>

<commit_message>
Deployed f95eef55 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/en/Manual/source/tab/connectors.xlsx
+++ b/en/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,8 +22,8 @@
     <sheet name="X3_M1_6pin_BLZP" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="X4_M2_6pin_BLZP" sheetId="13" state="visible" r:id="rId15"/>
     <sheet name="X1_24V_5pin_Microlock" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="X3_DCbus_2pin_pressfit" sheetId="15" state="visible" r:id="rId17"/>
-    <sheet name="X3_M1_3pin_pressfit" sheetId="16" state="visible" r:id="rId18"/>
+    <sheet name="X2_DCbus_2pin_pressfit" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="X2_M1_3pin_pressfit" sheetId="16" state="visible" r:id="rId18"/>
     <sheet name="X4_BR_4pin_Microlock" sheetId="17" state="visible" r:id="rId19"/>
     <sheet name="X2_DCbus_3pin_wago_2636" sheetId="18" state="visible" r:id="rId20"/>
     <sheet name="X3_M1_4pin_wago_2626" sheetId="19" state="visible" r:id="rId21"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="585">
   <si>
     <t xml:space="preserve">This is a workbook with source tables of TGZ/TGS connector descriptions in English. Each sheet corresponds to one unique connector type. Since connectors are often repeated within TGZ (typically those on the control board), they are only listed once. I.e. E.g. IO connector 22pin weidmuller B2CF is used over and over again, so it is only listed here once as "X8_IO_22pin_B2CF"</t>
   </si>
@@ -1390,10 +1390,16 @@
     <t xml:space="preserve">0V</t>
   </si>
   <si>
+    <t xml:space="preserve">PT1000_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">0~5V</t>
   </si>
   <si>
-    <t xml:space="preserve">HALL_IN1</t>
+    <t xml:space="preserve">PT1000_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HALL1</t>
   </si>
   <si>
     <t xml:space="preserve">Hall 1 signal</t>
@@ -1402,31 +1408,31 @@
     <t xml:space="preserve">5~30V</t>
   </si>
   <si>
-    <t xml:space="preserve">GNDHALL</t>
+    <t xml:space="preserve">HGND</t>
   </si>
   <si>
     <t xml:space="preserve">Hall common ground</t>
   </si>
   <si>
-    <t xml:space="preserve">HALL_IN2</t>
+    <t xml:space="preserve">HALL2</t>
   </si>
   <si>
     <t xml:space="preserve">Hall 2 signal</t>
   </si>
   <si>
-    <t xml:space="preserve">VCCHALL</t>
+    <t xml:space="preserve">VHO</t>
   </si>
   <si>
     <t xml:space="preserve">Hall output power (fused)</t>
   </si>
   <si>
-    <t xml:space="preserve">HALL_IN3</t>
+    <t xml:space="preserve">HALL3</t>
   </si>
   <si>
     <t xml:space="preserve">Hall 3 signal</t>
   </si>
   <si>
-    <t xml:space="preserve">VCCHALL_IN</t>
+    <t xml:space="preserve">VHI</t>
   </si>
   <si>
     <t xml:space="preserve">Hall input power</t>
@@ -2230,7 +2236,7 @@
             <v>#X10_CAN_4pin_B2CF</v>
           </cell>
           <cell r="B4" t="str">
-            <v>B2CF 3.50/04/180 SN OR BX</v>
+            <v>B2CF 3.50/04/180 SN OR BX </v>
           </cell>
           <cell r="C4" t="str">
             <v>Weidmüller</v>
@@ -2244,7 +2250,7 @@
             <v>#X6_FB1_8pin_B2CF</v>
           </cell>
           <cell r="B5" t="str">
-            <v>B2CF 3.50/08/180 SN OR BX</v>
+            <v>B2CF 3.50/08/180 SN OR BX </v>
           </cell>
           <cell r="C5" t="str">
             <v>Weidmüller</v>
@@ -2258,7 +2264,7 @@
             <v>#X7_FB2_8pin_B2CF</v>
           </cell>
           <cell r="B6" t="str">
-            <v>B2CF 3.50/08/180 SN OR BX</v>
+            <v>B2CF 3.50/08/180 SN OR BX </v>
           </cell>
           <cell r="C6" t="str">
             <v>Weidmüller</v>
@@ -2272,7 +2278,7 @@
             <v>#X5_FBE_12pin_B2CF</v>
           </cell>
           <cell r="B7" t="str">
-            <v>B2CF 3.50/12/180 SN OR BX</v>
+            <v>B2CF 3.50/12/180 SN OR BX </v>
           </cell>
           <cell r="C7" t="str">
             <v>Weidmüller</v>
@@ -2286,7 +2292,7 @@
             <v>#X1_24V_5pin_BCZ</v>
           </cell>
           <cell r="B8" t="str">
-            <v>BCZ 3.81/05/180 SN OR BX</v>
+            <v>BCZ 3.81/05/180 SN OR BX </v>
           </cell>
           <cell r="C8" t="str">
             <v>Weidmüller</v>
@@ -2300,7 +2306,7 @@
             <v>#X3_M1_6pin_BLZP</v>
           </cell>
           <cell r="B9" t="str">
-            <v>BLZP 5.08HC/06/180 SN OR BX</v>
+            <v>BLZP 5.08HC/06/180 SN OR BX </v>
           </cell>
           <cell r="C9" t="str">
             <v>Weidmüller</v>
@@ -2314,7 +2320,7 @@
             <v>#X4_M2_6pin_BLZP</v>
           </cell>
           <cell r="B10" t="str">
-            <v>BLZP 5.08HC/06/180 SN OR BX</v>
+            <v>BLZP 5.08HC/06/180 SN OR BX </v>
           </cell>
           <cell r="C10" t="str">
             <v>Weidmüller</v>
@@ -2328,7 +2334,7 @@
             <v>#X2_48_DC_1778065</v>
           </cell>
           <cell r="B11" t="str">
-            <v>PC 5/ 2-STCL1-7,62</v>
+            <v>PC 5/ 2-STCL1-7,62 </v>
           </cell>
           <cell r="C11" t="str">
             <v>Phoenix Contact</v>
@@ -2342,7 +2348,7 @@
             <v>#X4_M1_6pin_SLS</v>
           </cell>
           <cell r="B12" t="str">
-            <v>SLS 5.08/06/180FI SN OR BX</v>
+            <v>SLS 5.08/06/180FI SN OR BX </v>
           </cell>
           <cell r="C12" t="str">
             <v>Weidmüller</v>
@@ -2356,7 +2362,7 @@
             <v>#X2_PWR_10pin_BLZP</v>
           </cell>
           <cell r="B13" t="str">
-            <v>BLZP 5.08HC/10/180 SN OR BX</v>
+            <v>BLZP 5.08HC/10/180 SN OR BX </v>
           </cell>
           <cell r="C13" t="str">
             <v>Weidmüller</v>
@@ -2370,7 +2376,7 @@
             <v>#X4_M1_6pin_BLF</v>
           </cell>
           <cell r="B14" t="str">
-            <v>BLF 7.62HP/06/180F</v>
+            <v>BLF 7.62HP/06/180F </v>
           </cell>
           <cell r="C14" t="str">
             <v>Weidmüller</v>
@@ -2384,7 +2390,7 @@
             <v>#X2_PWR_12pin_BLZ</v>
           </cell>
           <cell r="B15" t="str">
-            <v>BLZ 7.62HP/12/180F</v>
+            <v>BLZ 7.62HP/12/180F </v>
           </cell>
           <cell r="C15" t="str">
             <v>Weidmüller</v>
@@ -2398,7 +2404,7 @@
             <v>#X3_M1_4pin_wago_2636</v>
           </cell>
           <cell r="B16" t="str">
-            <v>PC 5/ 2-STCL1-7,62</v>
+            <v>PC 5/ 2-STCL1-7,62 </v>
           </cell>
           <cell r="C16" t="str">
             <v>Phoenix Contact</v>
@@ -2412,7 +2418,7 @@
             <v>#X4_M2_4pin_wago_2636</v>
           </cell>
           <cell r="B17" t="str">
-            <v>PC 5/ 2-STCL1-7,62</v>
+            <v>PC 5/ 2-STCL1-7,62 </v>
           </cell>
           <cell r="C17" t="str">
             <v>Phoenix Contact</v>
@@ -2468,7 +2474,7 @@
             <v>#X1_ACIN_PC5</v>
           </cell>
           <cell r="B21" t="str">
-            <v>PC 5/ 8-STCL1-7,62</v>
+            <v>PC 5/ 8-STCL1-7,62 </v>
           </cell>
           <cell r="C21" t="str">
             <v>Phoenix Contact</v>
@@ -2482,7 +2488,7 @@
             <v>#X2_DC_8pin_PC5</v>
           </cell>
           <cell r="B22" t="str">
-            <v>PC 5/ 8-STCL1-7,62</v>
+            <v>PC 5/ 8-STCL1-7,62 </v>
           </cell>
           <cell r="C22" t="str">
             <v>Phoenix Contact</v>
@@ -2496,7 +2502,7 @@
             <v>#X3_DO_4pin_BCZ</v>
           </cell>
           <cell r="B23" t="str">
-            <v>BCZ 3.81/04/180 SN BK BX</v>
+            <v>BCZ 3.81/04/180 SN BK BX </v>
           </cell>
           <cell r="C23" t="str">
             <v>Weidmüller</v>
@@ -2510,7 +2516,7 @@
             <v>#X3_24V_BLF_2_5</v>
           </cell>
           <cell r="B24" t="str">
-            <v>BLF 2.50/04/180 SN OR BX</v>
+            <v>BLF 2.50/04/180 SN OR BX </v>
           </cell>
           <cell r="C24" t="str">
             <v>Weidmüller</v>
@@ -2524,7 +2530,7 @@
             <v>#X10_CAN_4pin_B2CF</v>
           </cell>
           <cell r="B25" t="str">
-            <v>BCZ 3.81/04/180 SN OR BX</v>
+            <v>BCZ 3.81/04/180 SN OR BX </v>
           </cell>
           <cell r="C25" t="str">
             <v>Weidmüller</v>
@@ -2538,7 +2544,7 @@
             <v>#X5_DI_10pin_B2CF</v>
           </cell>
           <cell r="B26" t="str">
-            <v>B2CF 3.50/10/180 SN OR BX</v>
+            <v>B2CF 3.50/10/180 SN OR BX </v>
           </cell>
           <cell r="C26" t="str">
             <v>Weidmüller</v>
@@ -2552,7 +2558,7 @@
             <v>#X10_DO_10pin_B2CF</v>
           </cell>
           <cell r="B27" t="str">
-            <v>B2CF 3.50/10/180 SN OR BX</v>
+            <v>B2CF 3.50/10/180 SN OR BX </v>
           </cell>
           <cell r="C27" t="str">
             <v>Weidmüller</v>
@@ -2566,7 +2572,7 @@
             <v>#X1_24V_5pin_BCZ_TGM</v>
           </cell>
           <cell r="B28" t="str">
-            <v>BCZ 3.81/05/180 SN OR BX</v>
+            <v>BCZ 3.81/05/180 SN OR BX </v>
           </cell>
           <cell r="C28" t="str">
             <v>Weidmüller</v>
@@ -2580,7 +2586,7 @@
             <v>#X2_320_DC_1778078</v>
           </cell>
           <cell r="B29" t="str">
-            <v>PC 5/ 3-STCL1-7,62</v>
+            <v>PC 5/ 3-STCL1-7,62 </v>
           </cell>
           <cell r="C29" t="str">
             <v>Phoenix Contact</v>
@@ -2594,7 +2600,7 @@
             <v>#X6_FB1_8pin_B2CF_TGM</v>
           </cell>
           <cell r="B30" t="str">
-            <v>BCZ 3.81/08/180 SN OR BX</v>
+            <v>BCZ 3.81/08/180 SN OR BX </v>
           </cell>
           <cell r="C30" t="str">
             <v>Weidmüller</v>
@@ -2608,7 +2614,7 @@
             <v>#X7_FB2_8pin_B2CF_TGM</v>
           </cell>
           <cell r="B31" t="str">
-            <v>BCZ 3.81/08/180 SN OR BX</v>
+            <v>BCZ 3.81/08/180 SN OR BX </v>
           </cell>
           <cell r="C31" t="str">
             <v>Weidmüller</v>
@@ -2622,7 +2628,7 @@
             <v>#X5_FBE_12pin_B2CF_TGM</v>
           </cell>
           <cell r="B32" t="str">
-            <v>BCZ 3.81/12/180 SN OR BX</v>
+            <v>BCZ 3.81/12/180 SN OR BX </v>
           </cell>
           <cell r="C32" t="str">
             <v>Weidmüller</v>
@@ -2748,7 +2754,7 @@
             <v>#X2_560_DC_3pin_BLZ__7_62</v>
           </cell>
           <cell r="B41" t="str">
-            <v>BLZ 7.62HP/03/180LR SN BK BX</v>
+            <v>BLZ 7.62HP/03/180LR SN BK BX </v>
           </cell>
           <cell r="C41" t="str">
             <v>Weidmüller</v>
@@ -2762,7 +2768,7 @@
             <v>#X4_ACIN_4pin_TGS560_25</v>
           </cell>
           <cell r="B42" t="str">
-            <v>BVZ 7.62HP/04/180F SN BK BX</v>
+            <v>BVZ 7.62HP/04/180F SN BK BX </v>
           </cell>
           <cell r="C42" t="str">
             <v>Weidmüller</v>
@@ -2776,7 +2782,7 @@
             <v>#X1_DC_6pin_TGS560_25</v>
           </cell>
           <cell r="B43" t="str">
-            <v>BVZ 7.62HP/06/180F SN BK BX</v>
+            <v>BVZ 7.62HP/06/180F SN BK BX </v>
           </cell>
           <cell r="C43" t="str">
             <v>Weidmüller</v>
@@ -2790,7 +2796,7 @@
             <v>#X5_RBR_3pin_TGS560_25</v>
           </cell>
           <cell r="B44" t="str">
-            <v>BLZ 7.62HP/03/180F SN BK BX</v>
+            <v>BLZ 7.62HP/03/180F SN BK BX </v>
           </cell>
           <cell r="C44" t="str">
             <v>Weidmüller</v>
@@ -2804,7 +2810,7 @@
             <v>#S1_TGS560_DIP</v>
           </cell>
           <cell r="B45" t="str">
-            <v>DS03-254-04BE</v>
+            <v>DS03-254-04BE </v>
           </cell>
           <cell r="C45" t="str">
             <v>Same Sky</v>
@@ -2818,7 +2824,7 @@
             <v>#X4_TGS560_24V_5pin_BCZ</v>
           </cell>
           <cell r="B46" t="str">
-            <v>BCZ 3.81/05/180F SN OR BX</v>
+            <v>BCZ 3.81/05/180F SN OR BX </v>
           </cell>
           <cell r="C46" t="str">
             <v>Weidmüller</v>
@@ -2860,7 +2866,7 @@
             <v>#XBR_BR_6pin_BLF</v>
           </cell>
           <cell r="B49" t="str">
-            <v>BLF 5.00HC/06/180F SN OR BX          </v>
+            <v>BLF 5.00HC/06/180F SN OR BX           </v>
           </cell>
           <cell r="C49" t="str">
             <v>Weidmüller</v>
@@ -3169,7 +3175,7 @@
   <dimension ref="A1:L204"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I191" activeCellId="1" sqref="B4:C4 I191"/>
+      <selection pane="topLeft" activeCell="I191" activeCellId="0" sqref="I191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9247,7 +9253,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B4:C4 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9405,7 +9411,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9563,7 +9569,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B4:C4 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9693,7 +9699,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B4:C4 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9823,7 +9829,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="B4:C4 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9936,7 +9942,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="B4:C4 C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10009,8 +10015,8 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4:C4 B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10098,7 +10104,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10198,7 +10204,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="B4:C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10286,7 +10292,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10388,7 +10394,7 @@
   <dimension ref="A1:H260"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="B4:C4 B52"/>
+      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13519,7 +13525,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13621,7 +13627,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="B4:C4 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13751,7 +13757,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13862,10 +13868,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13945,10 +13951,6 @@
       <c r="D5" s="4" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -13969,7 +13971,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14069,7 +14071,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14141,7 +14143,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="B4:C4 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14271,7 +14273,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14457,7 +14459,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B4:C4 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14540,7 +14542,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14670,7 +14672,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4:C4 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14783,7 +14785,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="B4:C4 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14994,7 +14996,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15095,7 +15097,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="B4:C4 D9"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15197,7 +15199,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="1" sqref="B4:C4 E32"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15299,7 +15301,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15401,7 +15403,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15503,7 +15505,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15586,7 +15588,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="B4:C4 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15753,7 +15755,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15853,7 +15855,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15953,7 +15955,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="B4:C4 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16066,7 +16068,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="1" sqref="B4:C4 C18"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16225,7 +16227,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="B4:C4 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16384,7 +16386,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O42" activeCellId="1" sqref="B4:C4 O42"/>
+      <selection pane="topLeft" activeCell="O42" activeCellId="0" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16479,7 +16481,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16592,7 +16594,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="B4:C4 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16724,7 +16726,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T15" activeCellId="1" sqref="B4:C4 T15"/>
+      <selection pane="topLeft" activeCell="T15" activeCellId="0" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16855,7 +16857,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="1" sqref="B4:C4 C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16986,7 +16988,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="1" sqref="B4:C4 E20"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17240,7 +17242,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="B4:C4 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17493,7 +17495,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="B4:C4 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17746,7 +17748,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B4:C4 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17812,7 +17814,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17987,7 +17989,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B4:C4 D1"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18044,13 +18046,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>407</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18058,7 +18060,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>407</v>
@@ -18072,13 +18074,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>410</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18086,7 +18088,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>410</v>
@@ -18100,13 +18102,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18114,10 +18116,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>419</v>
@@ -18128,13 +18130,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18142,13 +18144,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18156,13 +18158,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18170,13 +18172,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18201,7 +18203,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="B4:C4 C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18230,7 +18232,7 @@
         <v>198</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18241,7 +18243,7 @@
         <v>196</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18252,7 +18254,7 @@
         <v>194</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18263,7 +18265,7 @@
         <v>192</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18274,7 +18276,7 @@
         <v>190</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18285,7 +18287,7 @@
         <v>188</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18296,7 +18298,7 @@
         <v>186</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18307,7 +18309,7 @@
         <v>184</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18315,10 +18317,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18326,10 +18328,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18337,10 +18339,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18348,10 +18350,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18362,7 +18364,7 @@
         <v>176</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18373,7 +18375,7 @@
         <v>174</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18384,7 +18386,7 @@
         <v>172</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18395,7 +18397,7 @@
         <v>170</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18406,7 +18408,7 @@
         <v>168</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18417,7 +18419,7 @@
         <v>166</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -18439,7 +18441,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="B4:C4 C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18465,10 +18467,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18476,10 +18478,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18487,10 +18489,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18498,10 +18500,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18509,10 +18511,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18520,10 +18522,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18531,10 +18533,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18542,10 +18544,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -18567,7 +18569,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="B4:C4 C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18593,10 +18595,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18604,10 +18606,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18618,7 +18620,7 @@
         <v>398</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18629,7 +18631,7 @@
         <v>397</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18637,10 +18639,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18651,7 +18653,7 @@
         <v>151</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18659,10 +18661,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18670,10 +18672,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18684,7 +18686,7 @@
         <v>397</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18695,7 +18697,7 @@
         <v>398</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18726,7 +18728,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18752,10 +18754,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18763,10 +18765,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18774,10 +18776,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18785,10 +18787,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18796,10 +18798,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18807,10 +18809,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18818,10 +18820,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18829,10 +18831,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18869,7 +18871,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18901,10 +18903,10 @@
         <v>316</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18915,10 +18917,10 @@
         <v>314</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18932,7 +18934,7 @@
         <v>313</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18946,7 +18948,7 @@
         <v>307</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18960,7 +18962,7 @@
         <v>309</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18974,7 +18976,7 @@
         <v>311</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18985,10 +18987,10 @@
         <v>241</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>494</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19025,7 +19027,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19054,10 +19056,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>324</v>
@@ -19068,10 +19070,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>324</v>
@@ -19126,7 +19128,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="1" sqref="B4:C4 I24"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19156,13 +19158,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19170,13 +19172,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>503</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19187,10 +19189,10 @@
         <v>147</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19204,7 +19206,7 @@
         <v>153</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19218,7 +19220,7 @@
         <v>152</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -19240,7 +19242,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="B4:C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19270,10 +19272,10 @@
         <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19284,10 +19286,10 @@
         <v>157</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19298,10 +19300,10 @@
         <v>241</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -19323,7 +19325,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19673,7 +19675,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="B4:C4 D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19705,10 +19707,10 @@
         <v>236</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19719,10 +19721,10 @@
         <v>239</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>508</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19736,7 +19738,7 @@
         <v>242</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19750,7 +19752,7 @@
         <v>244</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19764,7 +19766,7 @@
         <v>246</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19778,7 +19780,7 @@
         <v>248</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19803,7 +19805,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19835,10 +19837,10 @@
         <v>236</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19849,10 +19851,10 @@
         <v>239</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>508</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19866,7 +19868,7 @@
         <v>242</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19880,7 +19882,7 @@
         <v>244</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19894,7 +19896,7 @@
         <v>246</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19908,7 +19910,7 @@
         <v>248</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19933,7 +19935,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:C4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19949,7 +19951,7 @@
         <v>377</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>141</v>
@@ -19957,162 +19959,162 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>528</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>526</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="C18" s="12"/>
       <c r="H18" s="4"/>
@@ -20120,50 +20122,50 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="15"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="15"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="15"/>
@@ -20187,7 +20189,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="B4:C4 D18"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20200,10 +20202,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>141</v>
@@ -20211,107 +20213,107 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="15"/>
@@ -20323,7 +20325,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>141</v>
@@ -20333,20 +20335,20 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="15"/>
@@ -20402,7 +20404,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B4:C4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20434,10 +20436,10 @@
         <v>241</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20451,7 +20453,7 @@
         <v>307</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20465,7 +20467,7 @@
         <v>309</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20479,7 +20481,7 @@
         <v>311</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20516,7 +20518,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20548,10 +20550,10 @@
         <v>155</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20562,10 +20564,10 @@
         <v>157</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20576,10 +20578,10 @@
         <v>241</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20590,10 +20592,10 @@
         <v>155</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20604,10 +20606,10 @@
         <v>157</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20618,10 +20620,10 @@
         <v>241</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20661,7 +20663,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="1" sqref="B4:C4 E34"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20696,7 +20698,7 @@
         <v>313</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20707,10 +20709,10 @@
         <v>314</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20721,10 +20723,10 @@
         <v>316</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20764,7 +20766,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="B4:C4 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20794,10 +20796,10 @@
         <v>243</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20808,10 +20810,10 @@
         <v>245</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20822,10 +20824,10 @@
         <v>247</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>561</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20839,7 +20841,7 @@
         <v>156</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20853,7 +20855,7 @@
         <v>251</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -20875,7 +20877,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="B4:C4 D8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20905,10 +20907,10 @@
         <v>151</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20916,13 +20918,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>565</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20933,10 +20935,10 @@
         <v>230</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20947,10 +20949,10 @@
         <v>232</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20961,10 +20963,10 @@
         <v>151</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20978,7 +20980,7 @@
         <v>148</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -20992,7 +20994,7 @@
         <v>144</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21006,7 +21008,7 @@
         <v>146</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21017,10 +21019,10 @@
         <v>320</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21031,10 +21033,10 @@
         <v>318</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21092,7 +21094,7 @@
   <dimension ref="A1:C1009"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="1" sqref="B4:C4 J9"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21118,10 +21120,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21129,10 +21131,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21140,10 +21142,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21151,10 +21153,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21162,10 +21164,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21173,10 +21175,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21187,7 +21189,7 @@
         <v>159</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21198,7 +21200,7 @@
         <v>159</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24224,7 +24226,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="B4:C4 C11"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24322,7 +24324,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="B4:C4 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24373,7 +24375,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B4:C4 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>